<commit_message>
Mise à jour de l'application Streamlit
</commit_message>
<xml_diff>
--- a/data/Informations joueurs.xlsx
+++ b/data/Informations joueurs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophergallo/Desktop/Application perso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46267396-876B-1F4E-9C95-A1C7A1340304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3243FE-8B43-0F43-9193-A19FCCB22AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="500" windowWidth="10000" windowHeight="16380" xr2:uid="{88726A7A-4B88-8C42-AD00-6D2620F5EC74}"/>
+    <workbookView xWindow="18440" yWindow="500" windowWidth="10360" windowHeight="16380" xr2:uid="{88726A7A-4B88-8C42-AD00-6D2620F5EC74}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Date de naissance</t>
   </si>
@@ -134,9 +134,6 @@
     <t>BU</t>
   </si>
   <si>
-    <t>Amir</t>
-  </si>
-  <si>
     <t>Naim Dhib</t>
   </si>
   <si>
@@ -149,20 +146,56 @@
     <t>Ilyes Bougahnmi</t>
   </si>
   <si>
-    <t>Oumar</t>
+    <t>Amir Kherrab</t>
+  </si>
+  <si>
+    <t>1m82</t>
+  </si>
+  <si>
+    <t>1m70</t>
+  </si>
+  <si>
+    <t>1m84</t>
+  </si>
+  <si>
+    <t>1m78</t>
+  </si>
+  <si>
+    <t>1m83</t>
+  </si>
+  <si>
+    <t>1m77</t>
+  </si>
+  <si>
+    <t>Yoann Martelat</t>
+  </si>
+  <si>
+    <t>Omar Benyounes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,6 +232,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,7 +647,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,6 +797,9 @@
       <c r="D10" t="s">
         <v>27</v>
       </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -811,6 +856,9 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -825,6 +873,9 @@
       <c r="D15" t="s">
         <v>29</v>
       </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -840,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -854,7 +905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -867,8 +918,11 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -882,7 +936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -896,56 +950,121 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3">
+        <v>38447</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="B22">
+        <v>27</v>
+      </c>
+      <c r="C22" s="7">
+        <v>35850</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3">
+        <v>38918</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="C24" s="8">
+        <v>35921</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3">
+        <v>38223</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="3">
+        <v>36675</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27">
+        <v>28</v>
+      </c>
+      <c r="C27" s="7">
+        <v>35446</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A21:A26">
+  <conditionalFormatting sqref="A22:A27">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>

</xml_diff>